<commit_message>
add tests to read very large xlsx file (over 1 million rows) with ExcelStreamingItemReader; add tests to read rows with blank cells; modify ExcelStreamingItemReader to handle inlineStr cell value (as opposed to shared strings table).
</commit_message>
<xml_diff>
--- a/src/test/resources/person-movies.xlsx
+++ b/src/test/resources/person-movies.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Movies with Blank Cells" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="movies_2012" vbProcedure="false">Sheet2!$A$1:$D$101</definedName>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="343">
   <si>
     <t>rank</t>
   </si>
@@ -1154,20 +1155,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.83404255319149"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.8382978723404"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1617021276596"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.936170212766"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.83404255319149"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.6042553191489"/>
   </cols>
@@ -2600,12 +2601,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AK12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3903,4 +3904,94 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.60851063829787"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1914893617021"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.60851063829787"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>623357910</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>41033</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>41110</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>408010692</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>